<commit_message>
Create comparison of assigned OBS to reported ridership by route
</commit_message>
<xml_diff>
--- a/docs/data/input/obs_processing/reported_ridership.xlsx
+++ b/docs/data/input/obs_processing/reported_ridership.xlsx
@@ -4313,4 +4313,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC273F68D44EF549AD1BD0E5D55B5B7C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="315063b799ab555b4e77865ce3b3361e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35b81125-b047-47c8-b0b0-722baac7a528" xmlns:ns3="5fe89d89-77ff-4a7d-998d-403e04f568fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfebddd8dbdab9d9b5a54d21a7ba6ecf" ns2:_="" ns3:_="">
+    <xsd:import namespace="35b81125-b047-47c8-b0b0-722baac7a528"/>
+    <xsd:import namespace="5fe89d89-77ff-4a7d-998d-403e04f568fa"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="35b81125-b047-47c8-b0b0-722baac7a528" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5fe89d89-77ff-4a7d-998d-403e04f568fa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB43BCC-DE6F-4993-99E0-372BB5D3364D}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE3D8344-CC35-4281-88AA-D05B5401587C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C999541-36D5-43FB-9AD1-94217B2A4E83}"/>
 </file>
</xml_diff>